<commit_message>
re-run F1 and MCC evaluations with estimated threshold, give values of 0.000 for failed baselines, recalc metrics
</commit_message>
<xml_diff>
--- a/output_pkis1loto/metrics/pvalues_wilcoxon_rankSignTest.xlsx
+++ b/output_pkis1loto/metrics/pvalues_wilcoxon_rankSignTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Wilcoxon Sign Rank" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="16">
   <si>
     <t xml:space="preserve">ROCAUC</t>
   </si>
@@ -62,6 +62,12 @@
     <t xml:space="preserve">FASR10</t>
   </si>
   <si>
+    <t xml:space="preserve">F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCC</t>
+  </si>
+  <si>
     <t xml:space="preserve">nan</t>
   </si>
 </sst>
@@ -73,7 +79,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -118,6 +124,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFCE181E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFCE181E"/>
       <name val="Calibri"/>
@@ -133,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -197,6 +211,62 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -223,7 +293,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,15 +366,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -385,10 +495,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -942,6 +1052,360 @@
       </c>
       <c r="I29" s="1" t="n">
         <v>0.000200567324502567</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0.464244676020143</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>8.65681570462319E-006</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>9.83962088726811E-006</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>3.79006592094188E-022</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>2.76247360149094E-022</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>9.79683079102833E-020</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>2.15216002106861E-023</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>2.49807778090122E-023</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>6.92057144805701E-022</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0.00494736175138926</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>2.29135285529372E-024</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>2.10003751217147E-024</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>9.53100405701185E-024</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0.280816566057798</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>0.321608482189821</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="18" t="n">
+        <v>8.98309684571618E-026</v>
+      </c>
+      <c r="C37" s="19" t="n">
+        <v>1.09353095839858E-025</v>
+      </c>
+      <c r="D37" s="19" t="n">
+        <v>5.12071077512787E-024</v>
+      </c>
+      <c r="E37" s="19" t="n">
+        <v>0.00226818542539354</v>
+      </c>
+      <c r="F37" s="20" t="n">
+        <v>0.0254974172495684</v>
+      </c>
+      <c r="G37" s="21" t="n">
+        <v>0.0280250683426335</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="22" t="n">
+        <v>5.99420526091703E-028</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>1.99464006628441E-028</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>4.65646198111118E-026</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>6.32172752459088E-011</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>2.28002268507828E-009</v>
+      </c>
+      <c r="G38" s="23" t="n">
+        <v>2.64312111263079E-008</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>0.00562830724603902</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="24" t="n">
+        <v>1.76429544502534E-032</v>
+      </c>
+      <c r="C39" s="25" t="n">
+        <v>2.0897236285773E-032</v>
+      </c>
+      <c r="D39" s="25" t="n">
+        <v>2.64968668306575E-031</v>
+      </c>
+      <c r="E39" s="25" t="n">
+        <v>3.14283171242192E-016</v>
+      </c>
+      <c r="F39" s="25" t="n">
+        <v>1.7921420688374E-014</v>
+      </c>
+      <c r="G39" s="26" t="n">
+        <v>1.1628148637628E-013</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>3.5876432043283E-009</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>0.000402585257262448</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>0.485531154301245</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>0.16259547139169</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>0.0940186728359833</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>1.96734455374724E-022</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>5.62580843027512E-022</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>1.26958086775765E-020</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>7.10779155877084E-024</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>2.11960141860554E-024</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>5.97744764658385E-023</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>0.00527128607509469</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>2.5432934727829E-024</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>3.07623500794991E-024</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>1.74385091232439E-024</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>0.443248861889435</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>0.220241195168975</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="18" t="n">
+        <v>1.0699584945166E-025</v>
+      </c>
+      <c r="C47" s="19" t="n">
+        <v>1.15586193163621E-025</v>
+      </c>
+      <c r="D47" s="19" t="n">
+        <v>2.47315516473569E-024</v>
+      </c>
+      <c r="E47" s="19" t="n">
+        <v>0.00174393150822375</v>
+      </c>
+      <c r="F47" s="20" t="n">
+        <v>0.0280380634345934</v>
+      </c>
+      <c r="G47" s="21" t="n">
+        <v>0.0296934317762956</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="22" t="n">
+        <v>9.23698368865501E-028</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>3.21727017629808E-028</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>3.493159030973E-026</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>8.7727870532796E-011</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>3.61136585891729E-009</v>
+      </c>
+      <c r="G48" s="23" t="n">
+        <v>2.12664998248445E-008</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <v>0.00695380217068244</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="24" t="n">
+        <v>1.92293454852495E-032</v>
+      </c>
+      <c r="C49" s="25" t="n">
+        <v>1.18549607955468E-032</v>
+      </c>
+      <c r="D49" s="25" t="n">
+        <v>1.63051753632238E-031</v>
+      </c>
+      <c r="E49" s="25" t="n">
+        <v>1.66109654726528E-015</v>
+      </c>
+      <c r="F49" s="25" t="n">
+        <v>1.07555150807617E-013</v>
+      </c>
+      <c r="G49" s="26" t="n">
+        <v>5.31951170668108E-013</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>8.2422892603313E-009</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>0.00125093877541172</v>
       </c>
     </row>
   </sheetData>
@@ -962,14 +1426,14 @@
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="18" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="27" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -977,28 +1441,28 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="27" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="0" t="s">
@@ -1013,7 +1477,7 @@
         <v>0.713505040262249</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1055,7 +1519,7 @@
         <v>2.62333828783256E-018</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1105,7 +1569,7 @@
         <v>0.15893266120082</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1150,13 +1614,13 @@
       <c r="D8" s="9" t="n">
         <v>1.25536396348077E-020</v>
       </c>
-      <c r="E8" s="10" t="n">
+      <c r="E8" s="28" t="n">
         <v>0.0463301869404211</v>
       </c>
-      <c r="F8" s="19" t="n">
+      <c r="F8" s="29" t="n">
         <v>0.0529945507397423</v>
       </c>
-      <c r="G8" s="20" t="n">
+      <c r="G8" s="30" t="n">
         <v>0.0138511721952983</v>
       </c>
       <c r="H8" s="1" t="n">
@@ -1510,13 +1974,13 @@
         <v>2.59148446597482E-018</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1539,10 +2003,10 @@
         <v>0.0707204535424769</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1568,7 +2032,7 @@
         <v>0.986410956645745</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>

</xml_diff>